<commit_message>
Updated for EXIOBASE 3.9.4 public release
</commit_message>
<xml_diff>
--- a/data/00_auxiliary/other/emis_conv_char.xlsx
+++ b/data/00_auxiliary/other/emis_conv_char.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kajwanr\Projects\cafean_python\data\auxiliary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kajwa\work\code\cafean\data\00_auxiliary\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9401D81A-6B66-4934-B480-704A4C8445BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C947206-AEBA-47BA-8F86-156A65DD9BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26205" yWindow="1395" windowWidth="19980" windowHeight="19215" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="2775" windowWidth="28020" windowHeight="15285" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
   <si>
     <t>Emission definitions and characterization</t>
   </si>
@@ -232,10 +232,19 @@
     <t>Bio CO2 are not included in the total GHG</t>
   </si>
   <si>
-    <t>CO2_bio</t>
+    <t>New combustion emission account</t>
   </si>
   <si>
-    <t>New combustion emission account</t>
+    <t>CO2 - combustion - air</t>
+  </si>
+  <si>
+    <t>CO2_bio - combustion - air</t>
+  </si>
+  <si>
+    <t>N2O - combustion - air</t>
+  </si>
+  <si>
+    <t>CH4 - combustion - air</t>
   </si>
 </sst>
 </file>
@@ -795,7 +804,7 @@
   <dimension ref="A1:AMI1019"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,7 +1552,7 @@
     </row>
     <row r="21" spans="1:1019" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
@@ -1558,7 +1567,7 @@
         <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y21" s="3"/>
       <c r="AD21" s="3"/>
@@ -1603,7 +1612,7 @@
     </row>
     <row r="22" spans="1:1019" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>35</v>
@@ -1618,7 +1627,7 @@
         <v>29</v>
       </c>
       <c r="F22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AD22" s="3"/>
       <c r="BN22" s="3"/>
@@ -1655,7 +1664,7 @@
     </row>
     <row r="23" spans="1:1019" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
@@ -1670,12 +1679,12 @@
         <v>29</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1019" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
@@ -1690,7 +1699,7 @@
         <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="QA24" s="3"/>
       <c r="ST24" s="3"/>

</xml_diff>